<commit_message>
feat:filled ranks dictionary, added corresponded sheet to dictionaries.xlsx for reference
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/dictionaries.xlsx
+++ b/renderer/dictionaries/dictionaries.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396DA217-451B-DF4B-BAE1-DE4996F18179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C19AEA-DD18-1843-8B41-880BE89B0F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{18F3DDB0-F3B0-4042-A2E8-682B46F64E38}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{18F3DDB0-F3B0-4042-A2E8-682B46F64E38}"/>
   </bookViews>
   <sheets>
     <sheet name="Посади" sheetId="3" r:id="rId1"/>
     <sheet name="Підрозділи" sheetId="4" r:id="rId2"/>
     <sheet name="Військовослужбовці" sheetId="1" r:id="rId3"/>
+    <sheet name="Військові звання" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>старший науковий співробітник</t>
   </si>
@@ -211,6 +212,138 @@
   </si>
   <si>
     <t>ж</t>
+  </si>
+  <si>
+    <t>Відповідник rank листа військовослужбовці</t>
+  </si>
+  <si>
+    <t>Звання</t>
+  </si>
+  <si>
+    <t>працівник Збройних Сил України</t>
+  </si>
+  <si>
+    <t>курсант</t>
+  </si>
+  <si>
+    <t>рекрут</t>
+  </si>
+  <si>
+    <t>солдат</t>
+  </si>
+  <si>
+    <t>матрос</t>
+  </si>
+  <si>
+    <t>старший солдат</t>
+  </si>
+  <si>
+    <t>старший матрос</t>
+  </si>
+  <si>
+    <t>молодший сержант</t>
+  </si>
+  <si>
+    <t>старшина 2 статті</t>
+  </si>
+  <si>
+    <t>сержант</t>
+  </si>
+  <si>
+    <t>старшина 1 статті</t>
+  </si>
+  <si>
+    <t>старший сержант</t>
+  </si>
+  <si>
+    <t>головний старшина</t>
+  </si>
+  <si>
+    <t>головний сержант</t>
+  </si>
+  <si>
+    <t>головний корабельний старшина</t>
+  </si>
+  <si>
+    <t>штаб-сержант</t>
+  </si>
+  <si>
+    <t>штаб-старшина</t>
+  </si>
+  <si>
+    <t>майстер-сержант</t>
+  </si>
+  <si>
+    <t>майстер-старшина</t>
+  </si>
+  <si>
+    <t>старший майстер-сержант</t>
+  </si>
+  <si>
+    <t>старший майстер-старшина</t>
+  </si>
+  <si>
+    <t>головний майстер-сержант</t>
+  </si>
+  <si>
+    <t>головний майстер-старшина</t>
+  </si>
+  <si>
+    <t>молодший лейтенант</t>
+  </si>
+  <si>
+    <t>лейтенант</t>
+  </si>
+  <si>
+    <t>старший лейтенант</t>
+  </si>
+  <si>
+    <t>капітан</t>
+  </si>
+  <si>
+    <t>капітан-лейтенант</t>
+  </si>
+  <si>
+    <t>майор</t>
+  </si>
+  <si>
+    <t>капітан 3 рангу</t>
+  </si>
+  <si>
+    <t>підполковник</t>
+  </si>
+  <si>
+    <t>капітан 2 рангу</t>
+  </si>
+  <si>
+    <t>полковник</t>
+  </si>
+  <si>
+    <t>капітан 1 рангу</t>
+  </si>
+  <si>
+    <t>бригадний генерал</t>
+  </si>
+  <si>
+    <t>коммодор</t>
+  </si>
+  <si>
+    <t>генерал-майор</t>
+  </si>
+  <si>
+    <t>контрадмірал</t>
+  </si>
+  <si>
+    <t>генерал-лейтенант</t>
+  </si>
+  <si>
+    <t>віцеадмірал</t>
+  </si>
+  <si>
+    <t>генерал</t>
+  </si>
+  <si>
+    <t>адмірал</t>
   </si>
 </sst>
 </file>
@@ -276,13 +409,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BAAE4B9-3FEE-D84B-B8AA-F9DF1EBE136A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -915,4 +1057,367 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031D30DC-FAA3-094A-8A2D-8F816709740C}">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="31" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="6">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="6">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="6">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="6">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="6">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="6">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="6">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="6">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="6">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="6">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="6">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="6">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="6">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="6">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="6">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="6">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="6">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="6">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="6">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="6">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="6">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="6">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="6">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="6">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat:added departure clauses generation + fixed some bugs
</commit_message>
<xml_diff>
--- a/renderer/dictionaries/dictionaries.xlsx
+++ b/renderer/dictionaries/dictionaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mykhailoaloshyn/Projects/Various/directive_generator/renderer/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C19AEA-DD18-1843-8B41-880BE89B0F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE2A14F-8DB5-E04F-B081-5903C47A1B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{18F3DDB0-F3B0-4042-A2E8-682B46F64E38}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{18F3DDB0-F3B0-4042-A2E8-682B46F64E38}"/>
   </bookViews>
   <sheets>
     <sheet name="Посади" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
   <si>
     <t>старший науковий співробітник</t>
   </si>
@@ -166,9 +166,6 @@
     <t>ІВАНОВА</t>
   </si>
   <si>
-    <t>A0000</t>
-  </si>
-  <si>
     <t>Олена Ігорівна</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>ГРАБОВУ</t>
   </si>
   <si>
-    <t>A1111</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -344,6 +338,24 @@
   </si>
   <si>
     <t>адмірал</t>
+  </si>
+  <si>
+    <t>first_name_genitive</t>
+  </si>
+  <si>
+    <t>last_name_genitive</t>
+  </si>
+  <si>
+    <t>Олени Ігорівни</t>
+  </si>
+  <si>
+    <t>ГРАБОВОЇ</t>
+  </si>
+  <si>
+    <t>військовій частині A0000</t>
+  </si>
+  <si>
+    <t>Міністерстві оборони України</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -752,7 +764,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
@@ -823,7 +835,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -914,65 +926,81 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2E3F80-3793-CA4E-A0A1-B472298AB53B}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="3" width="20" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="19" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="16.6640625" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="M1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -980,78 +1008,90 @@
         <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3">
-        <v>6</v>
+      <c r="I2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="M2" s="3">
         <v>1</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="N2" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="K3" s="3">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="5">
-        <v>6</v>
+      <c r="L3" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="M3" s="3">
         <v>4</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>50</v>
+      <c r="N3" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031D30DC-FAA3-094A-8A2D-8F816709740C}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1075,10 +1115,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1086,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1094,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1102,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1110,7 +1150,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1118,7 +1158,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1126,7 +1166,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1134,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1142,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1150,7 +1190,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1158,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1166,7 +1206,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1174,7 +1214,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1182,7 +1222,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1190,7 +1230,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1198,7 +1238,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1206,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1214,7 +1254,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1222,7 +1262,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1230,7 +1270,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1238,7 +1278,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1246,7 +1286,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1254,7 +1294,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1262,7 +1302,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1270,7 +1310,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1278,7 +1318,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1286,7 +1326,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1294,7 +1334,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1302,7 +1342,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1310,7 +1350,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1318,7 +1358,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1326,7 +1366,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1334,7 +1374,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1342,7 +1382,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1350,7 +1390,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1358,7 +1398,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1366,7 +1406,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1374,7 +1414,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1382,7 +1422,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1390,7 +1430,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1398,7 +1438,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1406,7 +1446,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1414,7 +1454,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>